<commit_message>
Update config for 6
</commit_message>
<xml_diff>
--- a/resources/cuprins/Cuprins Orchestra.xlsx
+++ b/resources/cuprins/Cuprins Orchestra.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\OBPP24\resources\cuprins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E557EE9E-9226-43F5-A0BB-FFB22ED294C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1683F8B-F5D3-49E6-BCF1-226EC282028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="112">
   <si>
     <t>Cântare</t>
   </si>
@@ -707,7 +708,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,13 +724,6 @@
     </font>
     <font>
       <sz val="7"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1014,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1069,9 +1063,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,6 +1078,809 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1734222159"/>
+        <c:axId val="1734232239"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1734222159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1734232239"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1734232239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1734222159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D0329119-6C9C-4F53-95E4-AEF4239F74BE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="61" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8660984" cy="6287541"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38ABFC4D-115C-5BEA-B3CA-EA39F34AD69A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1354,22 +2148,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="147" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="49.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="49.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +2183,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1399,7 +2193,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
@@ -1409,17 +2203,25 @@
       <c r="F4" s="6"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
@@ -1429,7 +2231,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
@@ -1439,17 +2241,25 @@
       <c r="F7" s="6"/>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
@@ -1467,7 +2277,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
@@ -1477,7 +2287,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +2297,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +2313,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="18" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +2323,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
@@ -1531,7 +2341,7 @@
       </c>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="18" t="s">
         <v>13</v>
       </c>
@@ -1541,7 +2351,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
@@ -1559,7 +2369,7 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="18" t="s">
         <v>15</v>
       </c>
@@ -1569,7 +2379,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
         <v>16</v>
       </c>
@@ -1579,7 +2389,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="18" t="s">
         <v>17</v>
       </c>
@@ -1589,7 +2399,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
@@ -1599,7 +2409,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="18" t="s">
         <v>19</v>
       </c>
@@ -1609,7 +2419,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="18" t="s">
         <v>20</v>
       </c>
@@ -1627,7 +2437,7 @@
       </c>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="18" t="s">
         <v>21</v>
       </c>
@@ -1645,7 +2455,7 @@
       </c>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="18" t="s">
         <v>22</v>
       </c>
@@ -1655,7 +2465,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="19"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="18" t="s">
         <v>23</v>
       </c>
@@ -1665,7 +2475,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="18" t="s">
         <v>24</v>
       </c>
@@ -1683,7 +2493,7 @@
       </c>
       <c r="G26" s="19"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="18" t="s">
         <v>25</v>
       </c>
@@ -1693,7 +2503,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="19"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="18" t="s">
         <v>26</v>
       </c>
@@ -1703,7 +2513,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="19"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="18" t="s">
         <v>27</v>
       </c>
@@ -1721,7 +2531,7 @@
       </c>
       <c r="G29" s="19"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="18" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +2541,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="18" t="s">
         <v>29</v>
       </c>
@@ -1741,7 +2551,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="18" t="s">
         <v>30</v>
       </c>
@@ -1751,7 +2561,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="19"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +2571,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="19"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="18" t="s">
         <v>32</v>
       </c>
@@ -1771,7 +2581,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="18" t="s">
         <v>33</v>
       </c>
@@ -1781,7 +2591,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="19"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" s="18" t="s">
         <v>34</v>
       </c>
@@ -1791,7 +2601,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="19"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="18" t="s">
         <v>35</v>
       </c>
@@ -1801,7 +2611,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="19"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" s="18" t="s">
         <v>36</v>
       </c>
@@ -1811,7 +2621,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="19"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="18" t="s">
         <v>37</v>
       </c>
@@ -1821,7 +2631,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="19"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" s="18" t="s">
         <v>38</v>
       </c>
@@ -1831,7 +2641,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="19"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="18" t="s">
         <v>39</v>
       </c>
@@ -1841,7 +2651,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="19"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" s="18" t="s">
         <v>40</v>
       </c>
@@ -1851,7 +2661,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="19"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="18" t="s">
         <v>41</v>
       </c>
@@ -1861,7 +2671,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="19"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" s="18" t="s">
         <v>42</v>
       </c>
@@ -1871,7 +2681,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="19"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" s="18" t="s">
         <v>43</v>
       </c>
@@ -1889,7 +2699,7 @@
       </c>
       <c r="G45" s="19"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="18" t="s">
         <v>44</v>
       </c>
@@ -1899,7 +2709,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="19"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="18" t="s">
         <v>45</v>
       </c>
@@ -1909,7 +2719,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="19"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B48" s="18" t="s">
         <v>46</v>
       </c>
@@ -1919,7 +2729,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="19"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" s="18" t="s">
         <v>47</v>
       </c>
@@ -1929,7 +2739,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="19"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" s="18" t="s">
         <v>48</v>
       </c>
@@ -1939,7 +2749,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="19"/>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="18" t="s">
         <v>49</v>
       </c>
@@ -1949,7 +2759,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="18" t="s">
         <v>50</v>
       </c>
@@ -1959,7 +2769,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="19"/>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" s="18" t="s">
         <v>51</v>
       </c>
@@ -1969,7 +2779,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="19"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" s="18" t="s">
         <v>52</v>
       </c>
@@ -1987,7 +2797,7 @@
       </c>
       <c r="G54" s="19"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" s="18" t="s">
         <v>53</v>
       </c>
@@ -1997,7 +2807,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="19"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" s="18" t="s">
         <v>54</v>
       </c>
@@ -2007,7 +2817,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="19"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" s="18" t="s">
         <v>55</v>
       </c>
@@ -2025,7 +2835,7 @@
       </c>
       <c r="G57" s="21"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" s="18" t="s">
         <v>56</v>
       </c>
@@ -2035,7 +2845,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="19"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" s="18" t="s">
         <v>57</v>
       </c>
@@ -2045,7 +2855,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" s="18" t="s">
         <v>58</v>
       </c>
@@ -2055,7 +2865,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="19"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" s="18" t="s">
         <v>59</v>
       </c>
@@ -2065,7 +2875,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="19"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" s="18" t="s">
         <v>60</v>
       </c>
@@ -2075,7 +2885,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="19"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" s="18" t="s">
         <v>61</v>
       </c>
@@ -2085,7 +2895,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="19"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" s="18" t="s">
         <v>62</v>
       </c>
@@ -2095,7 +2905,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="19"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" s="18" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2915,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="19"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" s="18" t="s">
         <v>64</v>
       </c>
@@ -2115,7 +2925,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="19"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" s="18" t="s">
         <v>65</v>
       </c>
@@ -2125,7 +2935,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" s="18" t="s">
         <v>66</v>
       </c>
@@ -2135,7 +2945,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="19"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" s="18" t="s">
         <v>67</v>
       </c>
@@ -2145,7 +2955,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="19"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" s="18" t="s">
         <v>68</v>
       </c>
@@ -2163,7 +2973,7 @@
       </c>
       <c r="G70" s="21"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" s="18" t="s">
         <v>69</v>
       </c>
@@ -2181,7 +2991,7 @@
       </c>
       <c r="G71" s="21"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B72" s="18" t="s">
         <v>70</v>
       </c>
@@ -2191,7 +3001,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="19"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B73" s="18" t="s">
         <v>71</v>
       </c>
@@ -2201,7 +3011,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="19"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B74" s="18" t="s">
         <v>72</v>
       </c>
@@ -2219,7 +3029,7 @@
       </c>
       <c r="G74" s="21"/>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B75" s="18" t="s">
         <v>73</v>
       </c>
@@ -2229,7 +3039,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="19"/>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B76" s="18" t="s">
         <v>74</v>
       </c>
@@ -2239,7 +3049,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="19"/>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B77" s="18" t="s">
         <v>75</v>
       </c>
@@ -2249,25 +3059,25 @@
       <c r="F77" s="6"/>
       <c r="G77" s="19"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B78" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D78" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F78" s="24" t="s">
+      <c r="C78" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F78" s="15" t="s">
         <v>92</v>
       </c>
       <c r="G78" s="21"/>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B79" s="18" t="s">
         <v>77</v>
       </c>
@@ -2277,7 +3087,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="19"/>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B80" s="18" t="s">
         <v>78</v>
       </c>
@@ -2287,7 +3097,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="19"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B81" s="18" t="s">
         <v>79</v>
       </c>
@@ -2305,7 +3115,7 @@
       </c>
       <c r="G81" s="21"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B82" s="18" t="s">
         <v>80</v>
       </c>
@@ -2323,7 +3133,7 @@
       </c>
       <c r="G82" s="19"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B83" s="18" t="s">
         <v>81</v>
       </c>
@@ -2339,7 +3149,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="21"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B84" s="18" t="s">
         <v>82</v>
       </c>
@@ -2349,7 +3159,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="19"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B85" s="18" t="s">
         <v>83</v>
       </c>
@@ -2359,7 +3169,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="19"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B86" s="18" t="s">
         <v>84</v>
       </c>
@@ -2369,7 +3179,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="19"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B87" s="18" t="s">
         <v>111</v>
       </c>
@@ -2387,7 +3197,7 @@
       </c>
       <c r="G87" s="21"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B88" s="18" t="s">
         <v>85</v>
       </c>
@@ -2405,7 +3215,7 @@
       </c>
       <c r="G88" s="21"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B89" s="18" t="s">
         <v>86</v>
       </c>
@@ -2415,7 +3225,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="19"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B90" s="18" t="s">
         <v>87</v>
       </c>
@@ -2425,7 +3235,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="19"/>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B91" s="18" t="s">
         <v>93</v>
       </c>
@@ -2435,7 +3245,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="19"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B92" s="18" t="s">
         <v>94</v>
       </c>
@@ -2453,7 +3263,7 @@
       </c>
       <c r="G92" s="21"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B93" s="18" t="s">
         <v>95</v>
       </c>
@@ -2463,7 +3273,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="19"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B94" s="18" t="s">
         <v>96</v>
       </c>
@@ -2473,7 +3283,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="19"/>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B95" s="18" t="s">
         <v>97</v>
       </c>
@@ -2483,7 +3293,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="19"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B96" s="18" t="s">
         <v>98</v>
       </c>
@@ -2493,7 +3303,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="19"/>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" s="18" t="s">
         <v>99</v>
       </c>
@@ -2503,7 +3313,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="19"/>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" s="18" t="s">
         <v>100</v>
       </c>
@@ -2513,7 +3323,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="19"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" s="18" t="s">
         <v>101</v>
       </c>
@@ -2531,7 +3341,7 @@
       </c>
       <c r="G99" s="21"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" s="18" t="s">
         <v>109</v>
       </c>
@@ -2549,7 +3359,7 @@
       </c>
       <c r="G100" s="21"/>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" s="18" t="s">
         <v>110</v>
       </c>
@@ -2565,7 +3375,7 @@
       </c>
       <c r="G101" s="21"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" s="18" t="s">
         <v>102</v>
       </c>
@@ -2583,7 +3393,7 @@
       </c>
       <c r="G102" s="21"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" s="18" t="s">
         <v>103</v>
       </c>
@@ -2593,7 +3403,7 @@
       <c r="F103" s="6"/>
       <c r="G103" s="19"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" s="18" t="s">
         <v>104</v>
       </c>
@@ -2603,7 +3413,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="21"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" s="18" t="s">
         <v>105</v>
       </c>
@@ -2613,7 +3423,7 @@
       <c r="F105" s="6"/>
       <c r="G105" s="19"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" s="18" t="s">
         <v>106</v>
       </c>
@@ -2623,7 +3433,7 @@
       <c r="F106" s="6"/>
       <c r="G106" s="19"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" s="18" t="s">
         <v>107</v>
       </c>
@@ -2633,7 +3443,7 @@
       <c r="F107" s="6"/>
       <c r="G107" s="19"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B108" s="19"/>
       <c r="C108" s="13"/>
       <c r="D108" s="5"/>
@@ -2641,7 +3451,7 @@
       <c r="F108" s="6"/>
       <c r="G108" s="19"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" s="19"/>
       <c r="C109" s="13"/>
       <c r="D109" s="5"/>
@@ -2649,7 +3459,7 @@
       <c r="F109" s="6"/>
       <c r="G109" s="19"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B110" s="19"/>
       <c r="C110" s="13"/>
       <c r="D110" s="5"/>
@@ -2657,7 +3467,7 @@
       <c r="F110" s="6"/>
       <c r="G110" s="19"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B111" s="19"/>
       <c r="C111" s="13"/>
       <c r="D111" s="5"/>
@@ -2665,7 +3475,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="19"/>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B112" s="19"/>
       <c r="C112" s="13"/>
       <c r="D112" s="5"/>
@@ -2673,7 +3483,7 @@
       <c r="F112" s="6"/>
       <c r="G112" s="19"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113" s="19"/>
       <c r="C113" s="13"/>
       <c r="D113" s="5"/>
@@ -2681,7 +3491,7 @@
       <c r="F113" s="6"/>
       <c r="G113" s="19"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B114" s="19"/>
       <c r="C114" s="13"/>
       <c r="D114" s="5"/>
@@ -2689,7 +3499,7 @@
       <c r="F114" s="6"/>
       <c r="G114" s="19"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B115" s="19"/>
       <c r="C115" s="13"/>
       <c r="D115" s="5"/>
@@ -2697,7 +3507,7 @@
       <c r="F115" s="6"/>
       <c r="G115" s="19"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B116" s="19"/>
       <c r="C116" s="13"/>
       <c r="D116" s="5"/>
@@ -2705,7 +3515,7 @@
       <c r="F116" s="6"/>
       <c r="G116" s="19"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B117" s="19"/>
       <c r="C117" s="13"/>
       <c r="D117" s="5"/>
@@ -2713,7 +3523,7 @@
       <c r="F117" s="6"/>
       <c r="G117" s="19"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B118" s="19"/>
       <c r="C118" s="13"/>
       <c r="D118" s="5"/>
@@ -2721,7 +3531,7 @@
       <c r="F118" s="6"/>
       <c r="G118" s="19"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B119" s="19"/>
       <c r="C119" s="13"/>
       <c r="D119" s="5"/>
@@ -2729,7 +3539,7 @@
       <c r="F119" s="6"/>
       <c r="G119" s="19"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B120" s="19"/>
       <c r="C120" s="13"/>
       <c r="D120" s="5"/>
@@ -2737,7 +3547,7 @@
       <c r="F120" s="6"/>
       <c r="G120" s="19"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B121" s="19"/>
       <c r="C121" s="13"/>
       <c r="D121" s="5"/>
@@ -2745,7 +3555,7 @@
       <c r="F121" s="6"/>
       <c r="G121" s="19"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B122" s="19"/>
       <c r="C122" s="13"/>
       <c r="D122" s="5"/>
@@ -2753,7 +3563,7 @@
       <c r="F122" s="6"/>
       <c r="G122" s="19"/>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B123" s="19"/>
       <c r="C123" s="13"/>
       <c r="D123" s="5"/>
@@ -2761,7 +3571,7 @@
       <c r="F123" s="6"/>
       <c r="G123" s="19"/>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B124" s="19"/>
       <c r="C124" s="13"/>
       <c r="D124" s="5"/>
@@ -2769,7 +3579,7 @@
       <c r="F124" s="6"/>
       <c r="G124" s="19"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B125" s="19"/>
       <c r="C125" s="13"/>
       <c r="D125" s="5"/>
@@ -2777,7 +3587,7 @@
       <c r="F125" s="6"/>
       <c r="G125" s="19"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B126" s="19"/>
       <c r="C126" s="13"/>
       <c r="D126" s="5"/>
@@ -2785,7 +3595,7 @@
       <c r="F126" s="6"/>
       <c r="G126" s="19"/>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B127" s="19"/>
       <c r="C127" s="13"/>
       <c r="D127" s="5"/>
@@ -2793,7 +3603,7 @@
       <c r="F127" s="6"/>
       <c r="G127" s="19"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128" s="19"/>
       <c r="C128" s="13"/>
       <c r="D128" s="5"/>
@@ -2801,7 +3611,7 @@
       <c r="F128" s="6"/>
       <c r="G128" s="19"/>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129" s="19"/>
       <c r="C129" s="13"/>
       <c r="D129" s="5"/>
@@ -2809,7 +3619,7 @@
       <c r="F129" s="6"/>
       <c r="G129" s="19"/>
     </row>
-    <row r="130" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B130" s="20"/>
       <c r="C130" s="16"/>
       <c r="D130" s="7"/>

</xml_diff>

<commit_message>
Update 27, add 30, 35
</commit_message>
<xml_diff>
--- a/resources/cuprins/Cuprins Orchestra.xlsx
+++ b/resources/cuprins/Cuprins Orchestra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\OBPP24\resources\cuprins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F251554C-95D2-49CD-A629-F6CAAD03FA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B87C9-D165-43A7-9F30-231D247E3271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="124">
   <si>
     <t>Cântare</t>
   </si>
@@ -1736,32 +1736,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
-    <col min="2" max="2" width="49.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1796875" style="1"/>
-    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.81640625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="49.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="34" t="s">
         <v>111</v>
       </c>
       <c r="I2" s="35"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="L4" s="28"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
@@ -1849,7 +1849,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1865,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1881,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>6</v>
       </c>
@@ -1905,7 +1905,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>7</v>
       </c>
@@ -1929,7 +1929,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
@@ -1945,7 +1945,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>9</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="L12" s="5"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>10</v>
       </c>
@@ -1983,7 +1983,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>12</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>13</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>14</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>15</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>16</v>
       </c>
@@ -2095,7 +2095,7 @@
       <c r="L19" s="5"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>17</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>18</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="L21" s="5"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>20</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="L23" s="5"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>21</v>
       </c>
@@ -2207,7 +2207,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>22</v>
       </c>
@@ -2223,7 +2223,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>23</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>24</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
         <v>25</v>
       </c>
@@ -2279,7 +2279,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>26</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>27</v>
       </c>
@@ -2319,7 +2319,7 @@
       <c r="L30" s="5"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>28</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="L31" s="5"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
         <v>29</v>
       </c>
@@ -2351,14 +2351,22 @@
       <c r="L32" s="5"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="G33" s="23"/>
       <c r="H33" s="30"/>
       <c r="I33" s="5"/>
@@ -2367,7 +2375,7 @@
       <c r="L33" s="5"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>31</v>
       </c>
@@ -2391,7 +2399,7 @@
       <c r="L34" s="5"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>32</v>
       </c>
@@ -2407,7 +2415,7 @@
       <c r="L35" s="5"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>33</v>
       </c>
@@ -2423,7 +2431,7 @@
       <c r="L36" s="5"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="18" t="s">
         <v>34</v>
       </c>
@@ -2438,7 +2446,7 @@
       <c r="L37" s="5"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="18" t="s">
         <v>35</v>
       </c>
@@ -2454,7 +2462,7 @@
       <c r="L38" s="5"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>36</v>
       </c>
@@ -2470,7 +2478,7 @@
       <c r="L39" s="5"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="18" t="s">
         <v>37</v>
       </c>
@@ -2486,7 +2494,7 @@
       <c r="L40" s="5"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2510,7 @@
       <c r="L41" s="5"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="18" t="s">
         <v>39</v>
       </c>
@@ -2518,7 +2526,7 @@
       <c r="L42" s="5"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="18" t="s">
         <v>40</v>
       </c>
@@ -2534,7 +2542,7 @@
       <c r="L43" s="5"/>
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>41</v>
       </c>
@@ -2550,7 +2558,7 @@
       <c r="L44" s="5"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>42</v>
       </c>
@@ -2566,7 +2574,7 @@
       <c r="L45" s="5"/>
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>43</v>
       </c>
@@ -2590,7 +2598,7 @@
       <c r="L46" s="5"/>
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>44</v>
       </c>
@@ -2606,7 +2614,7 @@
       <c r="L47" s="5"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
         <v>45</v>
       </c>
@@ -2622,7 +2630,7 @@
       <c r="L48" s="5"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>46</v>
       </c>
@@ -2638,7 +2646,7 @@
       <c r="L49" s="5"/>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>47</v>
       </c>
@@ -2654,7 +2662,7 @@
       <c r="L50" s="5"/>
       <c r="M50" s="6"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>48</v>
       </c>
@@ -2670,7 +2678,7 @@
       <c r="L51" s="5"/>
       <c r="M51" s="6"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="18" t="s">
         <v>49</v>
       </c>
@@ -2686,7 +2694,7 @@
       <c r="L52" s="5"/>
       <c r="M52" s="6"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="18" t="s">
         <v>50</v>
       </c>
@@ -2710,7 +2718,7 @@
       <c r="L53" s="5"/>
       <c r="M53" s="6"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
         <v>51</v>
       </c>
@@ -2726,7 +2734,7 @@
       <c r="L54" s="5"/>
       <c r="M54" s="6"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="18" t="s">
         <v>52</v>
       </c>
@@ -2750,7 +2758,7 @@
       <c r="L55" s="5"/>
       <c r="M55" s="6"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="18" t="s">
         <v>53</v>
       </c>
@@ -2766,7 +2774,7 @@
       <c r="L56" s="5"/>
       <c r="M56" s="6"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="18" t="s">
         <v>54</v>
       </c>
@@ -2790,7 +2798,7 @@
       <c r="L57" s="5"/>
       <c r="M57" s="6"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="18" t="s">
         <v>55</v>
       </c>
@@ -2814,7 +2822,7 @@
       <c r="L58" s="5"/>
       <c r="M58" s="6"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="18" t="s">
         <v>120</v>
       </c>
@@ -2838,7 +2846,7 @@
       <c r="L59" s="5"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
         <v>56</v>
       </c>
@@ -2854,7 +2862,7 @@
       <c r="L60" s="5"/>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="18" t="s">
         <v>57</v>
       </c>
@@ -2870,7 +2878,7 @@
       <c r="L61" s="5"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="18" t="s">
         <v>58</v>
       </c>
@@ -2886,7 +2894,7 @@
       <c r="L62" s="5"/>
       <c r="M62" s="6"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="18" t="s">
         <v>59</v>
       </c>
@@ -2902,7 +2910,7 @@
       <c r="L63" s="5"/>
       <c r="M63" s="6"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
         <v>60</v>
       </c>
@@ -2918,7 +2926,7 @@
       <c r="L64" s="5"/>
       <c r="M64" s="6"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
         <v>61</v>
       </c>
@@ -2934,7 +2942,7 @@
       <c r="L65" s="5"/>
       <c r="M65" s="6"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="18" t="s">
         <v>62</v>
       </c>
@@ -2950,7 +2958,7 @@
       <c r="L66" s="5"/>
       <c r="M66" s="6"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="18" t="s">
         <v>63</v>
       </c>
@@ -2966,7 +2974,7 @@
       <c r="L67" s="5"/>
       <c r="M67" s="6"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="18" t="s">
         <v>64</v>
       </c>
@@ -2982,7 +2990,7 @@
       <c r="L68" s="5"/>
       <c r="M68" s="6"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="18" t="s">
         <v>65</v>
       </c>
@@ -2998,7 +3006,7 @@
       <c r="L69" s="5"/>
       <c r="M69" s="6"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70" s="18" t="s">
         <v>66</v>
       </c>
@@ -3022,7 +3030,7 @@
       <c r="L70" s="5"/>
       <c r="M70" s="6"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
         <v>67</v>
       </c>
@@ -3046,7 +3054,7 @@
       <c r="L71" s="5"/>
       <c r="M71" s="6"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="18" t="s">
         <v>68</v>
       </c>
@@ -3062,7 +3070,7 @@
       <c r="L72" s="5"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73" s="18" t="s">
         <v>69</v>
       </c>
@@ -3078,7 +3086,7 @@
       <c r="L73" s="5"/>
       <c r="M73" s="6"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
         <v>70</v>
       </c>
@@ -3102,7 +3110,7 @@
       <c r="L74" s="5"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>71</v>
       </c>
@@ -3118,7 +3126,7 @@
       <c r="L75" s="5"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" s="18" t="s">
         <v>72</v>
       </c>
@@ -3134,7 +3142,7 @@
       <c r="L76" s="5"/>
       <c r="M76" s="6"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B77" s="18" t="s">
         <v>73</v>
       </c>
@@ -3150,7 +3158,7 @@
       <c r="L77" s="5"/>
       <c r="M77" s="6"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B78" s="18" t="s">
         <v>74</v>
       </c>
@@ -3174,7 +3182,7 @@
       <c r="L78" s="5"/>
       <c r="M78" s="6"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
         <v>75</v>
       </c>
@@ -3190,7 +3198,7 @@
       <c r="L79" s="5"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80" s="18" t="s">
         <v>76</v>
       </c>
@@ -3206,7 +3214,7 @@
       <c r="L80" s="5"/>
       <c r="M80" s="6"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
         <v>77</v>
       </c>
@@ -3230,7 +3238,7 @@
       <c r="L81" s="5"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B82" s="18" t="s">
         <v>78</v>
       </c>
@@ -3254,7 +3262,7 @@
       <c r="L82" s="5"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="18" t="s">
         <v>79</v>
       </c>
@@ -3276,7 +3284,7 @@
       <c r="L83" s="5"/>
       <c r="M83" s="6"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
         <v>80</v>
       </c>
@@ -3292,7 +3300,7 @@
       <c r="L84" s="5"/>
       <c r="M84" s="6"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B85" s="18" t="s">
         <v>81</v>
       </c>
@@ -3308,7 +3316,7 @@
       <c r="L85" s="5"/>
       <c r="M85" s="6"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
         <v>82</v>
       </c>
@@ -3324,7 +3332,7 @@
       <c r="L86" s="5"/>
       <c r="M86" s="6"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B87" s="18" t="s">
         <v>109</v>
       </c>
@@ -3348,7 +3356,7 @@
       <c r="L87" s="5"/>
       <c r="M87" s="6"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B88" s="18" t="s">
         <v>83</v>
       </c>
@@ -3372,7 +3380,7 @@
       <c r="L88" s="5"/>
       <c r="M88" s="6"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>84</v>
       </c>
@@ -3388,7 +3396,7 @@
       <c r="L89" s="5"/>
       <c r="M89" s="6"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>85</v>
       </c>
@@ -3404,7 +3412,7 @@
       <c r="L90" s="5"/>
       <c r="M90" s="6"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B91" s="18" t="s">
         <v>91</v>
       </c>
@@ -3420,7 +3428,7 @@
       <c r="L91" s="5"/>
       <c r="M91" s="6"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B92" s="18" t="s">
         <v>92</v>
       </c>
@@ -3444,7 +3452,7 @@
       <c r="L92" s="5"/>
       <c r="M92" s="6"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
         <v>93</v>
       </c>
@@ -3468,7 +3476,7 @@
       <c r="L93" s="5"/>
       <c r="M93" s="6"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B94" s="18" t="s">
         <v>94</v>
       </c>
@@ -3484,7 +3492,7 @@
       <c r="L94" s="5"/>
       <c r="M94" s="6"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B95" s="18" t="s">
         <v>95</v>
       </c>
@@ -3500,7 +3508,7 @@
       <c r="L95" s="5"/>
       <c r="M95" s="6"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B96" s="18" t="s">
         <v>96</v>
       </c>
@@ -3516,7 +3524,7 @@
       <c r="L96" s="5"/>
       <c r="M96" s="6"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
         <v>97</v>
       </c>
@@ -3532,7 +3540,7 @@
       <c r="L97" s="5"/>
       <c r="M97" s="6"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B98" s="18" t="s">
         <v>98</v>
       </c>
@@ -3548,7 +3556,7 @@
       <c r="L98" s="5"/>
       <c r="M98" s="6"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B99" s="18" t="s">
         <v>99</v>
       </c>
@@ -3572,7 +3580,7 @@
       <c r="L99" s="5"/>
       <c r="M99" s="6"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
         <v>107</v>
       </c>
@@ -3596,7 +3604,7 @@
       <c r="L100" s="5"/>
       <c r="M100" s="6"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B101" s="18" t="s">
         <v>108</v>
       </c>
@@ -3618,7 +3626,7 @@
       <c r="L101" s="5"/>
       <c r="M101" s="6"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B102" s="18" t="s">
         <v>100</v>
       </c>
@@ -3642,7 +3650,7 @@
       <c r="L102" s="5"/>
       <c r="M102" s="6"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B103" s="18" t="s">
         <v>101</v>
       </c>
@@ -3658,7 +3666,7 @@
       <c r="L103" s="5"/>
       <c r="M103" s="6"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
         <v>102</v>
       </c>
@@ -3674,7 +3682,7 @@
       <c r="L104" s="5"/>
       <c r="M104" s="6"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B105" s="18" t="s">
         <v>103</v>
       </c>
@@ -3690,7 +3698,7 @@
       <c r="L105" s="5"/>
       <c r="M105" s="6"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B106" s="18" t="s">
         <v>104</v>
       </c>
@@ -3706,7 +3714,7 @@
       <c r="L106" s="5"/>
       <c r="M106" s="6"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
         <v>105</v>
       </c>
@@ -3722,7 +3730,7 @@
       <c r="L107" s="5"/>
       <c r="M107" s="6"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B108" s="18" t="s">
         <v>110</v>
       </c>
@@ -3738,7 +3746,7 @@
       <c r="L108" s="5"/>
       <c r="M108" s="6"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B109" s="18" t="s">
         <v>114</v>
       </c>
@@ -3754,7 +3762,7 @@
       <c r="L109" s="5"/>
       <c r="M109" s="6"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B110" s="18" t="s">
         <v>115</v>
       </c>
@@ -3770,7 +3778,7 @@
       <c r="L110" s="5"/>
       <c r="M110" s="6"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
         <v>116</v>
       </c>
@@ -3786,7 +3794,7 @@
       <c r="L111" s="5"/>
       <c r="M111" s="6"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
         <v>121</v>
       </c>
@@ -3802,7 +3810,7 @@
       <c r="L112" s="5"/>
       <c r="M112" s="6"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B113" s="18" t="s">
         <v>117</v>
       </c>
@@ -3818,7 +3826,7 @@
       <c r="L113" s="5"/>
       <c r="M113" s="6"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B114" s="18" t="s">
         <v>123</v>
       </c>
@@ -3834,7 +3842,7 @@
       <c r="L114" s="5"/>
       <c r="M114" s="6"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
         <v>118</v>
       </c>
@@ -3850,7 +3858,7 @@
       <c r="L115" s="5"/>
       <c r="M115" s="6"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>119</v>
       </c>
@@ -3866,7 +3874,7 @@
       <c r="L116" s="5"/>
       <c r="M116" s="6"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B117" s="19"/>
       <c r="C117" s="13"/>
       <c r="D117" s="5"/>
@@ -3880,7 +3888,7 @@
       <c r="L117" s="5"/>
       <c r="M117" s="6"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B118" s="19"/>
       <c r="C118" s="13"/>
       <c r="D118" s="5"/>
@@ -3894,7 +3902,7 @@
       <c r="L118" s="5"/>
       <c r="M118" s="6"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B119" s="19"/>
       <c r="C119" s="13"/>
       <c r="D119" s="5"/>
@@ -3908,7 +3916,7 @@
       <c r="L119" s="5"/>
       <c r="M119" s="6"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B120" s="19"/>
       <c r="C120" s="13"/>
       <c r="D120" s="5"/>
@@ -3922,7 +3930,7 @@
       <c r="L120" s="5"/>
       <c r="M120" s="6"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B121" s="19"/>
       <c r="C121" s="13"/>
       <c r="D121" s="5"/>
@@ -3936,7 +3944,7 @@
       <c r="L121" s="5"/>
       <c r="M121" s="6"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B122" s="19"/>
       <c r="C122" s="13"/>
       <c r="D122" s="5"/>
@@ -3950,7 +3958,7 @@
       <c r="L122" s="5"/>
       <c r="M122" s="6"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B123" s="19"/>
       <c r="C123" s="13"/>
       <c r="D123" s="5"/>
@@ -3964,7 +3972,7 @@
       <c r="L123" s="5"/>
       <c r="M123" s="6"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B124" s="19"/>
       <c r="C124" s="13"/>
       <c r="D124" s="5"/>
@@ -3978,7 +3986,7 @@
       <c r="L124" s="5"/>
       <c r="M124" s="6"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B125" s="19"/>
       <c r="C125" s="13"/>
       <c r="D125" s="5"/>
@@ -3992,7 +4000,7 @@
       <c r="L125" s="5"/>
       <c r="M125" s="6"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B126" s="19"/>
       <c r="C126" s="13"/>
       <c r="D126" s="5"/>
@@ -4006,7 +4014,7 @@
       <c r="L126" s="5"/>
       <c r="M126" s="6"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B127" s="19"/>
       <c r="C127" s="13"/>
       <c r="D127" s="5"/>
@@ -4020,7 +4028,7 @@
       <c r="L127" s="5"/>
       <c r="M127" s="6"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B128" s="19"/>
       <c r="C128" s="13"/>
       <c r="D128" s="5"/>
@@ -4034,7 +4042,7 @@
       <c r="L128" s="5"/>
       <c r="M128" s="6"/>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B129" s="19"/>
       <c r="C129" s="13"/>
       <c r="D129" s="5"/>
@@ -4048,7 +4056,7 @@
       <c r="L129" s="5"/>
       <c r="M129" s="6"/>
     </row>
-    <row r="130" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="20"/>
       <c r="C130" s="16"/>
       <c r="D130" s="7"/>

</xml_diff>